<commit_message>
Rebuild Diagnostic Report FHIR IG - updated Base Organization and Organization with Mandatory Identifier
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/organization-dh-base-1.xlsx
+++ b/output/DiagnosticReport/organization-dh-base-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4020" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4020" uniqueCount="382">
   <si>
     <t>Path</t>
   </si>
@@ -146,7 +146,7 @@
     <t>*</t>
   </si>
   <si>
-    <t>An organisation in an Australian healthcare context</t>
+    <t>An organisation or an organisational unit</t>
   </si>
   <si>
     <t>A formally or informally recognized grouping of people or organizations formed for the purpose of achieving some form of collective action.  Includes companies, institutions, corporations, departments, community groups, healthcare practice groups, payer/insurer, etc.</t>
@@ -893,6 +893,9 @@
     <t>This resource is generally assumed to be active if no value is provided for the active element</t>
   </si>
   <si>
+    <t>true</t>
+  </si>
+  <si>
     <t>No equivalent in HL7 v2</t>
   </si>
   <si>
@@ -1055,7 +1058,7 @@
     <t>Organization.partOf</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/organization-dh-base-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/organization-dh-base-1)
 </t>
   </si>
   <si>
@@ -12329,7 +12332,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" hidden="true">
       <c r="A99" t="s" s="2">
         <v>273</v>
       </c>
@@ -12345,7 +12348,7 @@
         <v>49</v>
       </c>
       <c r="G99" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H99" t="s" s="2">
         <v>50</v>
@@ -12375,7 +12378,7 @@
         <v>279</v>
       </c>
       <c r="Q99" t="s" s="2">
-        <v>40</v>
+        <v>280</v>
       </c>
       <c r="R99" t="s" s="2">
         <v>40</v>
@@ -12432,21 +12435,21 @@
         <v>61</v>
       </c>
       <c r="AJ99" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AK99" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="AL99" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="AM99" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B100" s="2"/>
       <c r="C100" t="s" s="2">
@@ -12472,16 +12475,16 @@
         <v>143</v>
       </c>
       <c r="K100" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="L100" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="M100" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="N100" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="O100" t="s" s="2">
         <v>40</v>
@@ -12506,13 +12509,13 @@
         <v>40</v>
       </c>
       <c r="W100" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="X100" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="Y100" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="Z100" t="s" s="2">
         <v>40</v>
@@ -12530,7 +12533,7 @@
         <v>40</v>
       </c>
       <c r="AE100" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AF100" t="s" s="2">
         <v>41</v>
@@ -12545,21 +12548,21 @@
         <v>61</v>
       </c>
       <c r="AJ100" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="AK100" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AL100" t="s" s="2">
         <v>126</v>
       </c>
       <c r="AM100" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B101" s="2"/>
       <c r="C101" t="s" s="2">
@@ -12585,16 +12588,16 @@
         <v>51</v>
       </c>
       <c r="K101" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="L101" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="M101" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="N101" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="O101" t="s" s="2">
         <v>40</v>
@@ -12643,7 +12646,7 @@
         <v>40</v>
       </c>
       <c r="AE101" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AF101" t="s" s="2">
         <v>41</v>
@@ -12658,13 +12661,13 @@
         <v>61</v>
       </c>
       <c r="AJ101" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="AK101" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="AL101" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AM101" t="s" s="2">
         <v>40</v>
@@ -12672,7 +12675,7 @@
     </row>
     <row r="102">
       <c r="A102" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" t="s" s="2">
@@ -12698,16 +12701,16 @@
         <v>51</v>
       </c>
       <c r="K102" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="L102" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="M102" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="N102" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="O102" t="s" s="2">
         <v>40</v>
@@ -12756,7 +12759,7 @@
         <v>40</v>
       </c>
       <c r="AE102" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="AF102" t="s" s="2">
         <v>41</v>
@@ -12774,7 +12777,7 @@
         <v>40</v>
       </c>
       <c r="AK102" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="AL102" t="s" s="2">
         <v>40</v>
@@ -12785,7 +12788,7 @@
     </row>
     <row r="103">
       <c r="A103" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B103" s="2"/>
       <c r="C103" t="s" s="2">
@@ -12808,19 +12811,19 @@
         <v>40</v>
       </c>
       <c r="J103" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="K103" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="L103" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="M103" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="N103" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="O103" t="s" s="2">
         <v>40</v>
@@ -12869,7 +12872,7 @@
         <v>40</v>
       </c>
       <c r="AE103" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="AF103" t="s" s="2">
         <v>41</v>
@@ -12878,19 +12881,19 @@
         <v>42</v>
       </c>
       <c r="AH103" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="AI103" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="AJ103" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="AK103" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AL103" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AM103" t="s" s="2">
         <v>40</v>
@@ -12898,7 +12901,7 @@
     </row>
     <row r="104">
       <c r="A104" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B104" s="2"/>
       <c r="C104" t="s" s="2">
@@ -12921,19 +12924,19 @@
         <v>40</v>
       </c>
       <c r="J104" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="K104" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="L104" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="M104" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="N104" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="O104" t="s" s="2">
         <v>40</v>
@@ -12982,7 +12985,7 @@
         <v>40</v>
       </c>
       <c r="AE104" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AF104" t="s" s="2">
         <v>41</v>
@@ -12991,19 +12994,19 @@
         <v>42</v>
       </c>
       <c r="AH104" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="AI104" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="AJ104" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="AK104" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="AL104" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AM104" t="s" s="2">
         <v>40</v>
@@ -13011,7 +13014,7 @@
     </row>
     <row r="105">
       <c r="A105" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B105" s="2"/>
       <c r="C105" t="s" s="2">
@@ -13034,17 +13037,17 @@
         <v>50</v>
       </c>
       <c r="J105" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="K105" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="L105" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="M105" s="2"/>
       <c r="N105" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O105" t="s" s="2">
         <v>40</v>
@@ -13093,7 +13096,7 @@
         <v>40</v>
       </c>
       <c r="AE105" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="AF105" t="s" s="2">
         <v>41</v>
@@ -13108,10 +13111,10 @@
         <v>61</v>
       </c>
       <c r="AJ105" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AK105" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="AL105" t="s" s="2">
         <v>126</v>
@@ -13122,7 +13125,7 @@
     </row>
     <row r="106">
       <c r="A106" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B106" s="2"/>
       <c r="C106" t="s" s="2">
@@ -13145,19 +13148,19 @@
         <v>40</v>
       </c>
       <c r="J106" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K106" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="L106" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="M106" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="N106" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="O106" t="s" s="2">
         <v>40</v>
@@ -13206,7 +13209,7 @@
         <v>40</v>
       </c>
       <c r="AE106" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="AF106" t="s" s="2">
         <v>41</v>
@@ -13224,7 +13227,7 @@
         <v>40</v>
       </c>
       <c r="AK106" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="AL106" t="s" s="2">
         <v>40</v>
@@ -13235,7 +13238,7 @@
     </row>
     <row r="107" hidden="true">
       <c r="A107" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B107" s="2"/>
       <c r="C107" t="s" s="2">
@@ -13344,7 +13347,7 @@
     </row>
     <row r="108" hidden="true">
       <c r="A108" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B108" s="2"/>
       <c r="C108" t="s" s="2">
@@ -13455,11 +13458,11 @@
     </row>
     <row r="109" hidden="true">
       <c r="A109" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B109" s="2"/>
       <c r="C109" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D109" s="2"/>
       <c r="E109" t="s" s="2">
@@ -13481,10 +13484,10 @@
         <v>95</v>
       </c>
       <c r="K109" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="L109" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="M109" t="s" s="2">
         <v>98</v>
@@ -13539,7 +13542,7 @@
         <v>40</v>
       </c>
       <c r="AE109" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="AF109" t="s" s="2">
         <v>41</v>
@@ -13568,7 +13571,7 @@
     </row>
     <row r="110">
       <c r="A110" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B110" s="2"/>
       <c r="C110" t="s" s="2">
@@ -13594,14 +13597,14 @@
         <v>143</v>
       </c>
       <c r="K110" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="L110" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="M110" s="2"/>
       <c r="N110" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="O110" t="s" s="2">
         <v>40</v>
@@ -13629,10 +13632,10 @@
         <v>196</v>
       </c>
       <c r="X110" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="Y110" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="Z110" t="s" s="2">
         <v>40</v>
@@ -13650,7 +13653,7 @@
         <v>40</v>
       </c>
       <c r="AE110" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="AF110" t="s" s="2">
         <v>41</v>
@@ -13668,7 +13671,7 @@
         <v>40</v>
       </c>
       <c r="AK110" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="AL110" t="s" s="2">
         <v>40</v>
@@ -13679,7 +13682,7 @@
     </row>
     <row r="111">
       <c r="A111" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B111" s="2"/>
       <c r="C111" t="s" s="2">
@@ -13702,17 +13705,17 @@
         <v>40</v>
       </c>
       <c r="J111" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="K111" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="L111" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="M111" s="2"/>
       <c r="N111" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="O111" t="s" s="2">
         <v>40</v>
@@ -13761,7 +13764,7 @@
         <v>40</v>
       </c>
       <c r="AE111" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="AF111" t="s" s="2">
         <v>41</v>
@@ -13776,10 +13779,10 @@
         <v>61</v>
       </c>
       <c r="AJ111" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="AK111" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="AL111" t="s" s="2">
         <v>40</v>
@@ -13790,7 +13793,7 @@
     </row>
     <row r="112">
       <c r="A112" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B112" s="2"/>
       <c r="C112" t="s" s="2">
@@ -13813,17 +13816,17 @@
         <v>40</v>
       </c>
       <c r="J112" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="K112" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="L112" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="M112" s="2"/>
       <c r="N112" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="O112" t="s" s="2">
         <v>40</v>
@@ -13872,7 +13875,7 @@
         <v>40</v>
       </c>
       <c r="AE112" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="AF112" t="s" s="2">
         <v>41</v>
@@ -13887,10 +13890,10 @@
         <v>61</v>
       </c>
       <c r="AJ112" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="AK112" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AL112" t="s" s="2">
         <v>40</v>
@@ -13901,7 +13904,7 @@
     </row>
     <row r="113">
       <c r="A113" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B113" s="2"/>
       <c r="C113" t="s" s="2">
@@ -13924,17 +13927,17 @@
         <v>40</v>
       </c>
       <c r="J113" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="K113" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="L113" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="M113" s="2"/>
       <c r="N113" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="O113" t="s" s="2">
         <v>40</v>
@@ -13983,7 +13986,7 @@
         <v>40</v>
       </c>
       <c r="AE113" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="AF113" t="s" s="2">
         <v>41</v>
@@ -13998,10 +14001,10 @@
         <v>61</v>
       </c>
       <c r="AJ113" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="AK113" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AL113" t="s" s="2">
         <v>40</v>
@@ -14012,7 +14015,7 @@
     </row>
     <row r="114" hidden="true">
       <c r="A114" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B114" s="2"/>
       <c r="C114" t="s" s="2">
@@ -14035,17 +14038,17 @@
         <v>40</v>
       </c>
       <c r="J114" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="K114" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="L114" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="M114" s="2"/>
       <c r="N114" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="O114" t="s" s="2">
         <v>40</v>
@@ -14094,7 +14097,7 @@
         <v>40</v>
       </c>
       <c r="AE114" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AF114" t="s" s="2">
         <v>41</v>

</xml_diff>